<commit_message>
Actualizar proyecto: README mejorado, .gitignore optimizado y resultados actualizados
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,904 +454,794 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1.333214285714286</v>
       </c>
       <c r="B2" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>320</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.03333333333333333</v>
+        <v>1.366544642857143</v>
       </c>
       <c r="B3" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>320</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.06666666666666667</v>
+        <v>1.399875</v>
       </c>
       <c r="B4" t="n">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C4" t="n">
-        <v>320</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1</v>
+        <v>1.433205357142857</v>
       </c>
       <c r="B5" t="n">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C5" t="n">
-        <v>321</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1333333333333333</v>
+        <v>1.466535714285714</v>
       </c>
       <c r="B6" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C6" t="n">
-        <v>323</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1666666666666667</v>
+        <v>1.499866071428572</v>
       </c>
       <c r="B7" t="n">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C7" t="n">
-        <v>326</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.2</v>
+        <v>1.533196428571429</v>
       </c>
       <c r="B8" t="n">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C8" t="n">
-        <v>329</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.2333333333333333</v>
+        <v>1.566526785714286</v>
       </c>
       <c r="B9" t="n">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C9" t="n">
-        <v>330</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.2666666666666667</v>
+        <v>1.599857142857143</v>
       </c>
       <c r="B10" t="n">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C10" t="n">
-        <v>331</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.3</v>
+        <v>1.6331875</v>
       </c>
       <c r="B11" t="n">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="C11" t="n">
-        <v>331</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.3333333333333333</v>
+        <v>1.666517857142857</v>
       </c>
       <c r="B12" t="n">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="C12" t="n">
-        <v>327</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.3666666666666666</v>
+        <v>1.699848214285715</v>
       </c>
       <c r="B13" t="n">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="C13" t="n">
-        <v>321</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.4</v>
+        <v>1.733178571428572</v>
       </c>
       <c r="B14" t="n">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="C14" t="n">
-        <v>310</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.4333333333333333</v>
+        <v>1.766508928571429</v>
       </c>
       <c r="B15" t="n">
-        <v>104</v>
+        <v>165</v>
       </c>
       <c r="C15" t="n">
-        <v>291</v>
+        <v>388</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.4666666666666666</v>
+        <v>1.799839285714286</v>
       </c>
       <c r="B16" t="n">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="C16" t="n">
-        <v>258</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.4999999999999999</v>
+        <v>1.833169642857143</v>
       </c>
       <c r="B17" t="n">
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="C17" t="n">
-        <v>216</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.5333333333333333</v>
+        <v>1.8665</v>
       </c>
       <c r="B18" t="n">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C18" t="n">
-        <v>178</v>
+        <v>368</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.5666666666666667</v>
+        <v>1.899830357142857</v>
       </c>
       <c r="B19" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C19" t="n">
-        <v>144</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.6</v>
+        <v>1.933160714285715</v>
       </c>
       <c r="B20" t="n">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C20" t="n">
-        <v>116</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.6333333333333333</v>
+        <v>1.966491071428572</v>
       </c>
       <c r="B21" t="n">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="C21" t="n">
-        <v>93</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.999821428571429</v>
       </c>
       <c r="B22" t="n">
-        <v>253</v>
+        <v>210</v>
       </c>
       <c r="C22" t="n">
-        <v>75</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.7</v>
+        <v>2.033151785714286</v>
       </c>
       <c r="B23" t="n">
-        <v>273</v>
+        <v>216</v>
       </c>
       <c r="C23" t="n">
-        <v>61</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.7333333333333333</v>
+        <v>2.066482142857143</v>
       </c>
       <c r="B24" t="n">
-        <v>293</v>
+        <v>221</v>
       </c>
       <c r="C24" t="n">
-        <v>52</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.7666666666666666</v>
+        <v>2.0998125</v>
       </c>
       <c r="B25" t="n">
-        <v>312</v>
+        <v>226</v>
       </c>
       <c r="C25" t="n">
-        <v>49</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.7999999999999999</v>
+        <v>2.133142857142857</v>
       </c>
       <c r="B26" t="n">
-        <v>331</v>
+        <v>232</v>
       </c>
       <c r="C26" t="n">
-        <v>50</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.8333333333333333</v>
+        <v>2.166473214285713</v>
       </c>
       <c r="B27" t="n">
-        <v>351</v>
+        <v>236</v>
       </c>
       <c r="C27" t="n">
-        <v>56</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.8666666666666666</v>
+        <v>2.19980357142857</v>
       </c>
       <c r="B28" t="n">
-        <v>369</v>
+        <v>241</v>
       </c>
       <c r="C28" t="n">
-        <v>67</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.8999999999999999</v>
+        <v>2.233133928571427</v>
       </c>
       <c r="B29" t="n">
-        <v>387</v>
+        <v>246</v>
       </c>
       <c r="C29" t="n">
-        <v>80</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.9333333333333332</v>
+        <v>2.266464285714284</v>
       </c>
       <c r="B30" t="n">
-        <v>405</v>
+        <v>250</v>
       </c>
       <c r="C30" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.9666666666666666</v>
+        <v>2.299794642857141</v>
       </c>
       <c r="B31" t="n">
-        <v>422</v>
+        <v>254</v>
       </c>
       <c r="C31" t="n">
-        <v>125</v>
+        <v>437</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.9999999999999999</v>
+        <v>2.333124999999998</v>
       </c>
       <c r="B32" t="n">
-        <v>439</v>
+        <v>259</v>
       </c>
       <c r="C32" t="n">
-        <v>154</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1.033333333333333</v>
+        <v>2.366455357142855</v>
       </c>
       <c r="B33" t="n">
-        <v>455</v>
+        <v>262</v>
       </c>
       <c r="C33" t="n">
-        <v>187</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1.066666666666667</v>
+        <v>2.399785714285712</v>
       </c>
       <c r="B34" t="n">
-        <v>471</v>
+        <v>266</v>
       </c>
       <c r="C34" t="n">
-        <v>225</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1.1</v>
+        <v>2.433116071428569</v>
       </c>
       <c r="B35" t="n">
-        <v>486</v>
+        <v>270</v>
       </c>
       <c r="C35" t="n">
-        <v>265</v>
+        <v>362</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1.133333333333334</v>
+        <v>2.466446428571426</v>
       </c>
       <c r="B36" t="n">
-        <v>500</v>
+        <v>274</v>
       </c>
       <c r="C36" t="n">
-        <v>312</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1.166666666666667</v>
+        <v>2.499776785714283</v>
       </c>
       <c r="B37" t="n">
-        <v>514</v>
+        <v>277</v>
       </c>
       <c r="C37" t="n">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1.2</v>
+        <v>2.53310714285714</v>
       </c>
       <c r="B38" t="n">
-        <v>525</v>
+        <v>281</v>
       </c>
       <c r="C38" t="n">
-        <v>336</v>
+        <v>355</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1.233333333333334</v>
+        <v>2.566437499999997</v>
       </c>
       <c r="B39" t="n">
-        <v>533</v>
+        <v>284</v>
       </c>
       <c r="C39" t="n">
-        <v>304</v>
+        <v>364</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1.266666666666667</v>
+        <v>2.599767857142854</v>
       </c>
       <c r="B40" t="n">
-        <v>542</v>
+        <v>287</v>
       </c>
       <c r="C40" t="n">
-        <v>277</v>
+        <v>379</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1.300000000000001</v>
+        <v>2.63309821428571</v>
       </c>
       <c r="B41" t="n">
-        <v>550</v>
+        <v>291</v>
       </c>
       <c r="C41" t="n">
-        <v>256</v>
+        <v>399</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1.333333333333334</v>
+        <v>2.666428571428567</v>
       </c>
       <c r="B42" t="n">
-        <v>558</v>
+        <v>293</v>
       </c>
       <c r="C42" t="n">
-        <v>238</v>
+        <v>424</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1.366666666666668</v>
+        <v>2.699758928571424</v>
       </c>
       <c r="B43" t="n">
-        <v>566</v>
+        <v>296</v>
       </c>
       <c r="C43" t="n">
-        <v>226</v>
+        <v>448</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1.400000000000001</v>
+        <v>2.733089285714281</v>
       </c>
       <c r="B44" t="n">
-        <v>574</v>
+        <v>298</v>
       </c>
       <c r="C44" t="n">
-        <v>218</v>
+        <v>424</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1.433333333333334</v>
+        <v>2.766419642857138</v>
       </c>
       <c r="B45" t="n">
-        <v>583</v>
+        <v>301</v>
       </c>
       <c r="C45" t="n">
-        <v>214</v>
+        <v>408</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1.466666666666668</v>
+        <v>2.799749999999995</v>
       </c>
       <c r="B46" t="n">
-        <v>590</v>
+        <v>304</v>
       </c>
       <c r="C46" t="n">
-        <v>216</v>
+        <v>397</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1.500000000000001</v>
+        <v>2.833080357142852</v>
       </c>
       <c r="B47" t="n">
-        <v>598</v>
+        <v>306</v>
       </c>
       <c r="C47" t="n">
-        <v>222</v>
+        <v>392</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1.533333333333335</v>
+        <v>2.866410714285709</v>
       </c>
       <c r="B48" t="n">
-        <v>606</v>
+        <v>309</v>
       </c>
       <c r="C48" t="n">
-        <v>233</v>
+        <v>392</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1.566666666666668</v>
+        <v>2.899741071428566</v>
       </c>
       <c r="B49" t="n">
-        <v>613</v>
+        <v>311</v>
       </c>
       <c r="C49" t="n">
-        <v>249</v>
+        <v>398</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1.600000000000002</v>
+        <v>2.933071428571423</v>
       </c>
       <c r="B50" t="n">
-        <v>620</v>
+        <v>313</v>
       </c>
       <c r="C50" t="n">
-        <v>270</v>
+        <v>409</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1.633333333333335</v>
+        <v>2.96640178571428</v>
       </c>
       <c r="B51" t="n">
-        <v>627</v>
+        <v>315</v>
       </c>
       <c r="C51" t="n">
-        <v>296</v>
+        <v>426</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1.666666666666669</v>
+        <v>2.999732142857137</v>
       </c>
       <c r="B52" t="n">
-        <v>634</v>
+        <v>318</v>
       </c>
       <c r="C52" t="n">
-        <v>326</v>
+        <v>452</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1.700000000000002</v>
+        <v>3.033062499999994</v>
       </c>
       <c r="B53" t="n">
-        <v>639</v>
+        <v>320</v>
       </c>
       <c r="C53" t="n">
-        <v>360</v>
+        <v>441</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1.733333333333335</v>
+        <v>3.06639285714285</v>
       </c>
       <c r="B54" t="n">
-        <v>646</v>
+        <v>322</v>
       </c>
       <c r="C54" t="n">
-        <v>357</v>
+        <v>423</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1.766666666666669</v>
+        <v>3.099723214285707</v>
       </c>
       <c r="B55" t="n">
-        <v>653</v>
+        <v>324</v>
       </c>
       <c r="C55" t="n">
-        <v>335</v>
+        <v>415</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1.800000000000002</v>
+        <v>3.133053571428564</v>
       </c>
       <c r="B56" t="n">
-        <v>662</v>
+        <v>326</v>
       </c>
       <c r="C56" t="n">
-        <v>316</v>
+        <v>413</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1.833333333333336</v>
+        <v>3.166383928571421</v>
       </c>
       <c r="B57" t="n">
-        <v>670</v>
+        <v>328</v>
       </c>
       <c r="C57" t="n">
-        <v>302</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1.866666666666669</v>
+        <v>3.199714285714278</v>
       </c>
       <c r="B58" t="n">
-        <v>678</v>
+        <v>331</v>
       </c>
       <c r="C58" t="n">
-        <v>293</v>
+        <v>425</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1.900000000000003</v>
+        <v>3.233044642857135</v>
       </c>
       <c r="B59" t="n">
-        <v>685</v>
+        <v>333</v>
       </c>
       <c r="C59" t="n">
-        <v>289</v>
+        <v>443</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1.933333333333336</v>
+        <v>3.266374999999992</v>
       </c>
       <c r="B60" t="n">
-        <v>692</v>
+        <v>335</v>
       </c>
       <c r="C60" t="n">
-        <v>290</v>
+        <v>453</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1.966666666666669</v>
+        <v>3.299705357142849</v>
       </c>
       <c r="B61" t="n">
-        <v>699</v>
+        <v>337</v>
       </c>
       <c r="C61" t="n">
-        <v>295</v>
+        <v>440</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2.000000000000003</v>
+        <v>3.333035714285706</v>
       </c>
       <c r="B62" t="n">
-        <v>707</v>
+        <v>341</v>
       </c>
       <c r="C62" t="n">
-        <v>306</v>
+        <v>431</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2.033333333333336</v>
+        <v>3.366366071428563</v>
       </c>
       <c r="B63" t="n">
-        <v>714</v>
+        <v>343</v>
       </c>
       <c r="C63" t="n">
-        <v>321</v>
+        <v>429</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2.066666666666669</v>
+        <v>3.39969642857142</v>
       </c>
       <c r="B64" t="n">
-        <v>721</v>
+        <v>346</v>
       </c>
       <c r="C64" t="n">
-        <v>341</v>
+        <v>432</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2.100000000000002</v>
+        <v>3.433026785714277</v>
       </c>
       <c r="B65" t="n">
-        <v>728</v>
+        <v>349</v>
       </c>
       <c r="C65" t="n">
-        <v>365</v>
+        <v>444</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2.133333333333336</v>
+        <v>3.466357142857134</v>
       </c>
       <c r="B66" t="n">
-        <v>735</v>
+        <v>351</v>
       </c>
       <c r="C66" t="n">
-        <v>374</v>
+        <v>456</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2.166666666666669</v>
+        <v>3.499687499999991</v>
       </c>
       <c r="B67" t="n">
-        <v>743</v>
+        <v>353</v>
       </c>
       <c r="C67" t="n">
-        <v>356</v>
+        <v>451</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2.200000000000002</v>
+        <v>3.533017857142847</v>
       </c>
       <c r="B68" t="n">
-        <v>750</v>
+        <v>356</v>
       </c>
       <c r="C68" t="n">
-        <v>342</v>
+        <v>446</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2.233333333333335</v>
+        <v>3.566348214285704</v>
       </c>
       <c r="B69" t="n">
-        <v>758</v>
+        <v>357</v>
       </c>
       <c r="C69" t="n">
-        <v>335</v>
+        <v>446</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2.266666666666668</v>
+        <v>3.599678571428561</v>
       </c>
       <c r="B70" t="n">
-        <v>765</v>
+        <v>359</v>
       </c>
       <c r="C70" t="n">
-        <v>331</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2.300000000000002</v>
+        <v>3.633008928571418</v>
       </c>
       <c r="B71" t="n">
-        <v>773</v>
+        <v>361</v>
       </c>
       <c r="C71" t="n">
-        <v>332</v>
+        <v>457</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2.333333333333335</v>
+        <v>3.666339285714275</v>
       </c>
       <c r="B72" t="n">
-        <v>781</v>
+        <v>361</v>
       </c>
       <c r="C72" t="n">
-        <v>338</v>
+        <v>457</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2.366666666666668</v>
+        <v>3.699669642857132</v>
       </c>
       <c r="B73" t="n">
-        <v>788</v>
+        <v>361</v>
       </c>
       <c r="C73" t="n">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>2.400000000000001</v>
-      </c>
-      <c r="B74" t="n">
-        <v>795</v>
-      </c>
-      <c r="C74" t="n">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>2.433333333333334</v>
-      </c>
-      <c r="B75" t="n">
-        <v>802</v>
-      </c>
-      <c r="C75" t="n">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>2.466666666666668</v>
-      </c>
-      <c r="B76" t="n">
-        <v>810</v>
-      </c>
-      <c r="C76" t="n">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>2.500000000000001</v>
-      </c>
-      <c r="B77" t="n">
-        <v>818</v>
-      </c>
-      <c r="C77" t="n">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>2.533333333333334</v>
-      </c>
-      <c r="B78" t="n">
-        <v>825</v>
-      </c>
-      <c r="C78" t="n">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>2.566666666666667</v>
-      </c>
-      <c r="B79" t="n">
-        <v>830</v>
-      </c>
-      <c r="C79" t="n">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>2.600000000000001</v>
-      </c>
-      <c r="B80" t="n">
-        <v>834</v>
-      </c>
-      <c r="C80" t="n">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>2.633333333333334</v>
-      </c>
-      <c r="B81" t="n">
-        <v>837</v>
-      </c>
-      <c r="C81" t="n">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>2.666666666666667</v>
-      </c>
-      <c r="B82" t="n">
-        <v>841</v>
-      </c>
-      <c r="C82" t="n">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="B83" t="n">
-        <v>844</v>
-      </c>
-      <c r="C83" t="n">
-        <v>385</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -1365,7 +1255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1392,893 +1282,783 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.03333333333333333</v>
+        <v>1.366544642857143</v>
       </c>
       <c r="B2" t="n">
-        <v>-30</v>
+        <v>180.0160728636485</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>-420.0375033485132</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.06666666666666667</v>
+        <v>1.399875</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>240.0214304848647</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>-270.0241092954728</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1</v>
+        <v>1.433205357142857</v>
       </c>
       <c r="B4" t="n">
-        <v>-30</v>
+        <v>390.0348245379051</v>
       </c>
       <c r="C4" t="n">
-        <v>30</v>
+        <v>-90.00803643182425</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1333333333333333</v>
+        <v>1.466535714285714</v>
       </c>
       <c r="B5" t="n">
-        <v>-30</v>
+        <v>420.0375033485132</v>
       </c>
       <c r="C5" t="n">
-        <v>60</v>
+        <v>90.00803643182425</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.1666666666666667</v>
+        <v>1.499866071428572</v>
       </c>
       <c r="B6" t="n">
-        <v>-30</v>
+        <v>450.0401821591213</v>
       </c>
       <c r="C6" t="n">
-        <v>90</v>
+        <v>300.0267881060809</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.2</v>
+        <v>1.533196428571429</v>
       </c>
       <c r="B7" t="n">
-        <v>-60</v>
+        <v>420.0375033485132</v>
       </c>
       <c r="C7" t="n">
-        <v>90</v>
+        <v>450.0401821591213</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.2333333333333333</v>
+        <v>1.566526785714286</v>
       </c>
       <c r="B8" t="n">
-        <v>30</v>
+        <v>420.0375033485132</v>
       </c>
       <c r="C8" t="n">
-        <v>30</v>
+        <v>630.0562550227698</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.2666666666666667</v>
+        <v>1.599857142857143</v>
       </c>
       <c r="B9" t="n">
-        <v>60</v>
+        <v>450.0401821591213</v>
       </c>
       <c r="C9" t="n">
-        <v>30</v>
+        <v>780.0696490758103</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.3</v>
+        <v>1.6331875</v>
       </c>
       <c r="B10" t="n">
-        <v>150</v>
+        <v>390.0348245379051</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>960.0857219394587</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.3333333333333333</v>
+        <v>1.666517857142857</v>
       </c>
       <c r="B11" t="n">
-        <v>270</v>
+        <v>390.0348245379051</v>
       </c>
       <c r="C11" t="n">
-        <v>-120</v>
+        <v>1110.099115992499</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.3666666666666666</v>
+        <v>1.699848214285715</v>
       </c>
       <c r="B12" t="n">
-        <v>390</v>
+        <v>390.0348245379051</v>
       </c>
       <c r="C12" t="n">
-        <v>-180</v>
+        <v>1260.11251004554</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.4</v>
+        <v>1.733178571428572</v>
       </c>
       <c r="B13" t="n">
-        <v>510</v>
+        <v>330.0294669166889</v>
       </c>
       <c r="C13" t="n">
-        <v>-330</v>
+        <v>1410.12590409858</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.4333333333333333</v>
+        <v>1.766508928571429</v>
       </c>
       <c r="B14" t="n">
-        <v>600</v>
+        <v>360.032145727297</v>
       </c>
       <c r="C14" t="n">
-        <v>-570</v>
+        <v>1560.139298151621</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.4666666666666666</v>
+        <v>1.799839285714286</v>
       </c>
       <c r="B15" t="n">
-        <v>720</v>
+        <v>300.0267881060809</v>
       </c>
       <c r="C15" t="n">
-        <v>-990</v>
+        <v>1470.131261719796</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.4999999999999999</v>
+        <v>1.833169642857143</v>
       </c>
       <c r="B16" t="n">
-        <v>690</v>
+        <v>210.0187516742566</v>
       </c>
       <c r="C16" t="n">
-        <v>-1260</v>
+        <v>-1080.096437181891</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.5333333333333333</v>
+        <v>1.8665</v>
       </c>
       <c r="B17" t="n">
-        <v>630</v>
+        <v>180.0160728636485</v>
       </c>
       <c r="C17" t="n">
-        <v>-1140</v>
+        <v>-990.0884007500669</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.5666666666666667</v>
+        <v>1.899830357142857</v>
       </c>
       <c r="B18" t="n">
-        <v>630</v>
+        <v>180.0160728636485</v>
       </c>
       <c r="C18" t="n">
-        <v>-1020</v>
+        <v>-900.0803643182426</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.6</v>
+        <v>1.933160714285715</v>
       </c>
       <c r="B19" t="n">
-        <v>600</v>
+        <v>180.0160728636485</v>
       </c>
       <c r="C19" t="n">
-        <v>-840</v>
+        <v>-720.064291454594</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.6333333333333333</v>
+        <v>1.966491071428572</v>
       </c>
       <c r="B20" t="n">
-        <v>600</v>
+        <v>150.0133940530404</v>
       </c>
       <c r="C20" t="n">
-        <v>-690</v>
+        <v>-510.0455397803374</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.999821428571429</v>
       </c>
       <c r="B21" t="n">
-        <v>600</v>
+        <v>150.0133940530404</v>
       </c>
       <c r="C21" t="n">
-        <v>-540</v>
+        <v>-330.0294669166889</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.7</v>
+        <v>2.033151785714286</v>
       </c>
       <c r="B22" t="n">
-        <v>600</v>
+        <v>180.0160728636485</v>
       </c>
       <c r="C22" t="n">
-        <v>-420</v>
+        <v>-180.0160728636485</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.7333333333333333</v>
+        <v>2.066482142857143</v>
       </c>
       <c r="B23" t="n">
-        <v>600</v>
+        <v>150.0133940530404</v>
       </c>
       <c r="C23" t="n">
-        <v>-270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.7666666666666666</v>
+        <v>2.0998125</v>
       </c>
       <c r="B24" t="n">
-        <v>570</v>
+        <v>150.0133940530404</v>
       </c>
       <c r="C24" t="n">
-        <v>-90</v>
+        <v>180.0160728636485</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.7999999999999999</v>
+        <v>2.133142857142857</v>
       </c>
       <c r="B25" t="n">
-        <v>570</v>
+        <v>180.0160728636485</v>
       </c>
       <c r="C25" t="n">
-        <v>30</v>
+        <v>330.0294669166889</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.8333333333333333</v>
+        <v>2.166473214285713</v>
       </c>
       <c r="B26" t="n">
-        <v>600</v>
+        <v>120.0107152424323</v>
       </c>
       <c r="C26" t="n">
-        <v>180</v>
+        <v>510.0455397803374</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.8666666666666666</v>
+        <v>2.19980357142857</v>
       </c>
       <c r="B27" t="n">
-        <v>540</v>
+        <v>150.0133940530404</v>
       </c>
       <c r="C27" t="n">
-        <v>330</v>
+        <v>690.061612643986</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.8999999999999999</v>
+        <v>2.233133928571427</v>
       </c>
       <c r="B28" t="n">
-        <v>540</v>
+        <v>150.0133940530404</v>
       </c>
       <c r="C28" t="n">
-        <v>390</v>
+        <v>870.0776855076344</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.9333333333333332</v>
+        <v>2.266464285714284</v>
       </c>
       <c r="B29" t="n">
-        <v>540</v>
+        <v>120.0107152424323</v>
       </c>
       <c r="C29" t="n">
-        <v>600</v>
+        <v>1020.091079560675</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.9666666666666666</v>
+        <v>2.299794642857141</v>
       </c>
       <c r="B30" t="n">
-        <v>510</v>
+        <v>120.0107152424323</v>
       </c>
       <c r="C30" t="n">
-        <v>750</v>
+        <v>1110.099115992499</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.9999999999999999</v>
+        <v>2.333124999999998</v>
       </c>
       <c r="B31" t="n">
-        <v>510</v>
+        <v>150.0133940530404</v>
       </c>
       <c r="C31" t="n">
-        <v>870</v>
+        <v>-510.0455397803374</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1.033333333333333</v>
+        <v>2.366455357142855</v>
       </c>
       <c r="B32" t="n">
-        <v>480</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C32" t="n">
-        <v>990</v>
+        <v>-720.064291454594</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1.066666666666667</v>
+        <v>2.399785714285712</v>
       </c>
       <c r="B33" t="n">
-        <v>480</v>
+        <v>120.0107152424323</v>
       </c>
       <c r="C33" t="n">
-        <v>1140</v>
+        <v>-570.0508974015536</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1.1</v>
+        <v>2.433116071428569</v>
       </c>
       <c r="B34" t="n">
-        <v>450</v>
+        <v>120.0107152424323</v>
       </c>
       <c r="C34" t="n">
-        <v>1200</v>
+        <v>-450.0401821591213</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1.133333333333334</v>
+        <v>2.466446428571426</v>
       </c>
       <c r="B35" t="n">
-        <v>420</v>
+        <v>120.0107152424323</v>
       </c>
       <c r="C35" t="n">
-        <v>1410</v>
+        <v>-240.0214304848647</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1.166666666666667</v>
+        <v>2.499776785714283</v>
       </c>
       <c r="B36" t="n">
-        <v>420</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C36" t="n">
-        <v>1410</v>
+        <v>-60.00535762121617</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1.2</v>
+        <v>2.53310714285714</v>
       </c>
       <c r="B37" t="n">
-        <v>330</v>
+        <v>120.0107152424323</v>
       </c>
       <c r="C37" t="n">
-        <v>-690</v>
+        <v>90.00803643182425</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1.233333333333334</v>
+        <v>2.566437499999997</v>
       </c>
       <c r="B38" t="n">
-        <v>240</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C38" t="n">
-        <v>-960</v>
+        <v>270.0241092954728</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1.266666666666667</v>
+        <v>2.599767857142854</v>
       </c>
       <c r="B39" t="n">
-        <v>270</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C39" t="n">
-        <v>-810</v>
+        <v>450.0401821591213</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1.300000000000001</v>
+        <v>2.63309821428571</v>
       </c>
       <c r="B40" t="n">
-        <v>240</v>
+        <v>120.0107152424323</v>
       </c>
       <c r="C40" t="n">
-        <v>-630</v>
+        <v>600.0535762121617</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1.333333333333334</v>
+        <v>2.666428571428567</v>
       </c>
       <c r="B41" t="n">
-        <v>240</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C41" t="n">
-        <v>-540</v>
+        <v>750.0669702652021</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1.366666666666668</v>
+        <v>2.699758928571424</v>
       </c>
       <c r="B42" t="n">
-        <v>240</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C42" t="n">
-        <v>-360</v>
+        <v>720.064291454594</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1.400000000000001</v>
+        <v>2.733089285714281</v>
       </c>
       <c r="B43" t="n">
-        <v>240</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C43" t="n">
-        <v>-240</v>
+        <v>-720.064291454594</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1.433333333333334</v>
+        <v>2.766419642857138</v>
       </c>
       <c r="B44" t="n">
-        <v>270</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C44" t="n">
-        <v>-120</v>
+        <v>-480.0428609697294</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1.466666666666668</v>
+        <v>2.799749999999995</v>
       </c>
       <c r="B45" t="n">
-        <v>210</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C45" t="n">
-        <v>60</v>
+        <v>-330.0294669166889</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1.500000000000001</v>
+        <v>2.833080357142852</v>
       </c>
       <c r="B46" t="n">
-        <v>240</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C46" t="n">
-        <v>180</v>
+        <v>-150.0133940530404</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1.533333333333335</v>
+        <v>2.866410714285709</v>
       </c>
       <c r="B47" t="n">
-        <v>240</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C47" t="n">
-        <v>330</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1.566666666666668</v>
+        <v>2.899741071428566</v>
       </c>
       <c r="B48" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C48" t="n">
-        <v>480</v>
+        <v>180.0160728636485</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1.600000000000002</v>
+        <v>2.933071428571423</v>
       </c>
       <c r="B49" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C49" t="n">
-        <v>630</v>
+        <v>330.0294669166889</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1.633333333333335</v>
+        <v>2.96640178571428</v>
       </c>
       <c r="B50" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C50" t="n">
-        <v>780</v>
+        <v>510.0455397803374</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1.666666666666669</v>
+        <v>2.999732142857137</v>
       </c>
       <c r="B51" t="n">
-        <v>210</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C51" t="n">
-        <v>900</v>
+        <v>780.0696490758103</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1.700000000000002</v>
+        <v>3.033062499999994</v>
       </c>
       <c r="B52" t="n">
-        <v>150</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C52" t="n">
-        <v>1020</v>
+        <v>-330.0294669166889</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1.733333333333335</v>
+        <v>3.06639285714285</v>
       </c>
       <c r="B53" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C53" t="n">
-        <v>-90</v>
+        <v>-540.0482185909456</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1.766666666666669</v>
+        <v>3.099723214285707</v>
       </c>
       <c r="B54" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C54" t="n">
-        <v>-660</v>
+        <v>-240.0214304848647</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1.800000000000002</v>
+        <v>3.133053571428564</v>
       </c>
       <c r="B55" t="n">
-        <v>270</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C55" t="n">
-        <v>-570</v>
+        <v>-60.00535762121617</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1.833333333333336</v>
+        <v>3.166383928571421</v>
       </c>
       <c r="B56" t="n">
-        <v>240</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C56" t="n">
-        <v>-420</v>
+        <v>60.00535762121617</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1.866666666666669</v>
+        <v>3.199714285714278</v>
       </c>
       <c r="B57" t="n">
-        <v>240</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C57" t="n">
-        <v>-270</v>
+        <v>300.0267881060809</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1.900000000000003</v>
+        <v>3.233044642857135</v>
       </c>
       <c r="B58" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C58" t="n">
-        <v>-120</v>
+        <v>540.0482185909456</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1.933333333333336</v>
+        <v>3.266374999999992</v>
       </c>
       <c r="B59" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C59" t="n">
-        <v>30</v>
+        <v>300.0267881060809</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1.966666666666669</v>
+        <v>3.299705357142849</v>
       </c>
       <c r="B60" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C60" t="n">
-        <v>150</v>
+        <v>-390.0348245379051</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2.000000000000003</v>
+        <v>3.333035714285706</v>
       </c>
       <c r="B61" t="n">
-        <v>240</v>
+        <v>120.0107152424323</v>
       </c>
       <c r="C61" t="n">
-        <v>330</v>
+        <v>-270.0241092954728</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2.033333333333336</v>
+        <v>3.366366071428563</v>
       </c>
       <c r="B62" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C62" t="n">
-        <v>450</v>
+        <v>-60.00535762121617</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2.066666666666669</v>
+        <v>3.39969642857142</v>
       </c>
       <c r="B63" t="n">
-        <v>210</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C63" t="n">
-        <v>600</v>
+        <v>90.00803643182425</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2.100000000000002</v>
+        <v>3.433026785714277</v>
       </c>
       <c r="B64" t="n">
-        <v>210</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C64" t="n">
-        <v>720</v>
+        <v>360.032145727297</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2.133333333333336</v>
+        <v>3.466357142857134</v>
       </c>
       <c r="B65" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C65" t="n">
-        <v>270</v>
+        <v>360.032145727297</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2.166666666666669</v>
+        <v>3.499687499999991</v>
       </c>
       <c r="B66" t="n">
-        <v>240</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C66" t="n">
-        <v>-540</v>
+        <v>-150.0133940530404</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2.200000000000002</v>
+        <v>3.533017857142847</v>
       </c>
       <c r="B67" t="n">
-        <v>210</v>
+        <v>90.00803643182425</v>
       </c>
       <c r="C67" t="n">
-        <v>-420</v>
+        <v>-150.0133940530404</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2.233333333333335</v>
+        <v>3.566348214285704</v>
       </c>
       <c r="B68" t="n">
-        <v>240</v>
+        <v>30.00267881060809</v>
       </c>
       <c r="C68" t="n">
-        <v>-210</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2.266666666666668</v>
+        <v>3.599678571428561</v>
       </c>
       <c r="B69" t="n">
-        <v>210</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C69" t="n">
-        <v>-120</v>
+        <v>150.0133940530404</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2.300000000000002</v>
+        <v>3.633008928571418</v>
       </c>
       <c r="B70" t="n">
-        <v>240</v>
+        <v>60.00535762121617</v>
       </c>
       <c r="C70" t="n">
-        <v>30</v>
+        <v>180.0160728636485</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2.333333333333335</v>
+        <v>3.666339285714275</v>
       </c>
       <c r="B71" t="n">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2.366666666666668</v>
+        <v>3.699669642857132</v>
       </c>
       <c r="B72" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>2.400000000000001</v>
-      </c>
-      <c r="B73" t="n">
-        <v>210</v>
-      </c>
-      <c r="C73" t="n">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>2.433333333333334</v>
-      </c>
-      <c r="B74" t="n">
-        <v>210</v>
-      </c>
-      <c r="C74" t="n">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>2.466666666666668</v>
-      </c>
-      <c r="B75" t="n">
-        <v>240</v>
-      </c>
-      <c r="C75" t="n">
-        <v>-360</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>2.500000000000001</v>
-      </c>
-      <c r="B76" t="n">
-        <v>240</v>
-      </c>
-      <c r="C76" t="n">
-        <v>-330</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>2.533333333333334</v>
-      </c>
-      <c r="B77" t="n">
-        <v>210</v>
-      </c>
-      <c r="C77" t="n">
-        <v>-150</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>2.566666666666667</v>
-      </c>
-      <c r="B78" t="n">
-        <v>150</v>
-      </c>
-      <c r="C78" t="n">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>2.600000000000001</v>
-      </c>
-      <c r="B79" t="n">
-        <v>120</v>
-      </c>
-      <c r="C79" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>2.633333333333334</v>
-      </c>
-      <c r="B80" t="n">
-        <v>90</v>
-      </c>
-      <c r="C80" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>2.666666666666667</v>
-      </c>
-      <c r="B81" t="n">
-        <v>120</v>
-      </c>
-      <c r="C81" t="n">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="B82" t="n">
-        <v>90</v>
-      </c>
-      <c r="C82" t="n">
-        <v>-30</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2292,7 +2072,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2319,882 +2099,772 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.06666666666666667</v>
+        <v>1.399875</v>
       </c>
       <c r="B2" t="n">
-        <v>900</v>
+        <v>1800.321471625023</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.1</v>
+        <v>1.433205357142857</v>
       </c>
       <c r="B3" t="n">
-        <v>-900</v>
+        <v>4500.803679062558</v>
       </c>
       <c r="C3" t="n">
-        <v>900</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1333333333333333</v>
+        <v>1.466535714285714</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>900.1607358125111</v>
       </c>
       <c r="C4" t="n">
-        <v>900</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1666666666666667</v>
+        <v>1.499866071428572</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>900.1607358125111</v>
       </c>
       <c r="C5" t="n">
-        <v>900</v>
+        <v>6301.12515068758</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.2</v>
+        <v>1.533196428571429</v>
       </c>
       <c r="B6" t="n">
-        <v>-900</v>
+        <v>-900.1607358125111</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.2333333333333333</v>
+        <v>1.566526785714286</v>
       </c>
       <c r="B7" t="n">
-        <v>2700</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>-1800</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.2666666666666667</v>
+        <v>1.599857142857143</v>
       </c>
       <c r="B8" t="n">
-        <v>900</v>
+        <v>900.1607358125111</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.3</v>
+        <v>1.6331875</v>
       </c>
       <c r="B9" t="n">
-        <v>2700</v>
+        <v>-1800.321471625022</v>
       </c>
       <c r="C9" t="n">
-        <v>-900</v>
+        <v>5400.964414875067</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.3333333333333333</v>
+        <v>1.666517857142857</v>
       </c>
       <c r="B10" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>-3600</v>
+        <v>4500.80367906256</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.3666666666666666</v>
+        <v>1.699848214285715</v>
       </c>
       <c r="B11" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>-1800</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.4</v>
+        <v>1.733178571428572</v>
       </c>
       <c r="B12" t="n">
-        <v>3600</v>
+        <v>-1800.321471625024</v>
       </c>
       <c r="C12" t="n">
-        <v>-4500</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.4333333333333333</v>
+        <v>1.766508928571429</v>
       </c>
       <c r="B13" t="n">
-        <v>2700</v>
+        <v>900.1607358125111</v>
       </c>
       <c r="C13" t="n">
-        <v>-7200</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.4666666666666666</v>
+        <v>1.799839285714286</v>
       </c>
       <c r="B14" t="n">
-        <v>3600</v>
+        <v>-1800.321471625022</v>
       </c>
       <c r="C14" t="n">
-        <v>-12600</v>
+        <v>-2700.482207437538</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.4999999999999999</v>
+        <v>1.833169642857143</v>
       </c>
       <c r="B15" t="n">
-        <v>-900</v>
+        <v>-2700.482207437534</v>
       </c>
       <c r="C15" t="n">
-        <v>-8100</v>
+        <v>-76513.66254406347</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.5333333333333333</v>
+        <v>1.8665</v>
       </c>
       <c r="B16" t="n">
-        <v>-1800</v>
+        <v>-900.1607358125119</v>
       </c>
       <c r="C16" t="n">
-        <v>3600</v>
+        <v>2700.482207437535</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.5666666666666667</v>
+        <v>1.899830357142857</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>3600</v>
+        <v>2700.482207437535</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.6</v>
+        <v>1.933160714285715</v>
       </c>
       <c r="B18" t="n">
-        <v>-900</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>5400</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.6333333333333333</v>
+        <v>1.966491071428572</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>-900.1607358125111</v>
       </c>
       <c r="C19" t="n">
-        <v>4500</v>
+        <v>6301.12515068758</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.999821428571429</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>4500</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.7</v>
+        <v>2.033151785714286</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>900.1607358125111</v>
       </c>
       <c r="C21" t="n">
-        <v>3600</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.7333333333333333</v>
+        <v>2.066482142857143</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>-900.1607358125111</v>
       </c>
       <c r="C22" t="n">
-        <v>4500</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.7666666666666666</v>
+        <v>2.0998125</v>
       </c>
       <c r="B23" t="n">
-        <v>-900</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>5400</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.7999999999999999</v>
+        <v>2.133142857142857</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>900.1607358125111</v>
       </c>
       <c r="C24" t="n">
-        <v>3600</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.8333333333333333</v>
+        <v>2.166473214285713</v>
       </c>
       <c r="B25" t="n">
-        <v>900</v>
+        <v>-1800.321471625022</v>
       </c>
       <c r="C25" t="n">
-        <v>4500</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.8666666666666666</v>
+        <v>2.19980357142857</v>
       </c>
       <c r="B26" t="n">
-        <v>-1800</v>
+        <v>900.1607358125115</v>
       </c>
       <c r="C26" t="n">
-        <v>4500</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.8999999999999999</v>
+        <v>2.233133928571427</v>
       </c>
       <c r="B27" t="n">
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>1800</v>
+        <v>5400.964414875067</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.9333333333333332</v>
+        <v>2.266464285714284</v>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>-900.1607358125115</v>
       </c>
       <c r="C28" t="n">
-        <v>6300</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.9666666666666666</v>
+        <v>2.299794642857141</v>
       </c>
       <c r="B29" t="n">
-        <v>-900</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>4500</v>
+        <v>2700.482207437538</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.9999999999999999</v>
+        <v>2.333124999999998</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>900.1607358125115</v>
       </c>
       <c r="C30" t="n">
-        <v>3600</v>
+        <v>-48608.67973387562</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1.033333333333333</v>
+        <v>2.366455357142855</v>
       </c>
       <c r="B31" t="n">
-        <v>-900</v>
+        <v>-1800.321471625023</v>
       </c>
       <c r="C31" t="n">
-        <v>3600</v>
+        <v>-6301.12515068758</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1.066666666666667</v>
+        <v>2.399785714285712</v>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>900.1607358125115</v>
       </c>
       <c r="C32" t="n">
-        <v>4500</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1.1</v>
+        <v>2.433116071428569</v>
       </c>
       <c r="B33" t="n">
-        <v>-900</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>1800</v>
+        <v>3600.642943250044</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1.133333333333334</v>
+        <v>2.466446428571426</v>
       </c>
       <c r="B34" t="n">
-        <v>-900</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>6300</v>
+        <v>6301.12515068758</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1.166666666666667</v>
+        <v>2.499776785714283</v>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>-900.1607358125115</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1.2</v>
+        <v>2.53310714285714</v>
       </c>
       <c r="B36" t="n">
-        <v>-2700</v>
+        <v>900.1607358125115</v>
       </c>
       <c r="C36" t="n">
-        <v>-63000</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1.233333333333334</v>
+        <v>2.566437499999997</v>
       </c>
       <c r="B37" t="n">
-        <v>-2700</v>
+        <v>-900.1607358125115</v>
       </c>
       <c r="C37" t="n">
-        <v>-8100</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1.266666666666667</v>
+        <v>2.599767857142854</v>
       </c>
       <c r="B38" t="n">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>4500</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1.300000000000001</v>
+        <v>2.63309821428571</v>
       </c>
       <c r="B39" t="n">
-        <v>-900</v>
+        <v>900.1607358125115</v>
       </c>
       <c r="C39" t="n">
-        <v>5400</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1.333333333333334</v>
+        <v>2.666428571428567</v>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>-1800.321471625023</v>
       </c>
       <c r="C40" t="n">
-        <v>2700</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1.366666666666668</v>
+        <v>2.699758928571424</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>900.1607358125112</v>
       </c>
       <c r="C41" t="n">
-        <v>5400</v>
+        <v>-900.1607358125128</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1.400000000000001</v>
+        <v>2.733089285714281</v>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>-900.1607358125112</v>
       </c>
       <c r="C42" t="n">
-        <v>3600</v>
+        <v>-43207.71531900055</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1.433333333333334</v>
+        <v>2.766419642857138</v>
       </c>
       <c r="B43" t="n">
-        <v>900</v>
+        <v>900.1607358125112</v>
       </c>
       <c r="C43" t="n">
-        <v>3600</v>
+        <v>7201.28588650009</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1.466666666666668</v>
+        <v>2.799749999999995</v>
       </c>
       <c r="B44" t="n">
-        <v>-1800</v>
+        <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>5400</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1.500000000000001</v>
+        <v>2.833080357142852</v>
       </c>
       <c r="B45" t="n">
-        <v>900</v>
+        <v>-900.1607358125112</v>
       </c>
       <c r="C45" t="n">
-        <v>3600</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1.533333333333335</v>
+        <v>2.866410714285709</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>900.1607358125112</v>
       </c>
       <c r="C46" t="n">
-        <v>4500</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1.566666666666668</v>
+        <v>2.899741071428566</v>
       </c>
       <c r="B47" t="n">
-        <v>-900</v>
+        <v>-900.1607358125112</v>
       </c>
       <c r="C47" t="n">
-        <v>4500</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1.600000000000002</v>
+        <v>2.933071428571423</v>
       </c>
       <c r="B48" t="n">
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>4500</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1.633333333333335</v>
+        <v>2.96640178571428</v>
       </c>
       <c r="B49" t="n">
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>4500</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1.666666666666669</v>
+        <v>2.999732142857137</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>900.1607358125112</v>
       </c>
       <c r="C50" t="n">
-        <v>3600</v>
+        <v>8101.446622312605</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1.700000000000002</v>
+        <v>3.033062499999994</v>
       </c>
       <c r="B51" t="n">
-        <v>-1800</v>
+        <v>-900.1607358125112</v>
       </c>
       <c r="C51" t="n">
-        <v>3600</v>
+        <v>-33305.94722506293</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1.733333333333335</v>
+        <v>3.06639285714285</v>
       </c>
       <c r="B52" t="n">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>-33300</v>
+        <v>-6301.125150687581</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1.766666666666669</v>
+        <v>3.099723214285707</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>-17100</v>
+        <v>9001.607358125115</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1.800000000000002</v>
+        <v>3.133053571428564</v>
       </c>
       <c r="B54" t="n">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>2700</v>
+        <v>5400.964414875069</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1.833333333333336</v>
+        <v>3.166383928571421</v>
       </c>
       <c r="B55" t="n">
-        <v>-900</v>
+        <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>4500</v>
+        <v>3600.642943250045</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1.866666666666669</v>
+        <v>3.199714285714278</v>
       </c>
       <c r="B56" t="n">
-        <v>0</v>
+        <v>900.1607358125112</v>
       </c>
       <c r="C56" t="n">
-        <v>4500</v>
+        <v>7201.285886500091</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1.900000000000003</v>
+        <v>3.233044642857135</v>
       </c>
       <c r="B57" t="n">
-        <v>-900</v>
+        <v>-900.1607358125112</v>
       </c>
       <c r="C57" t="n">
-        <v>4500</v>
+        <v>7201.285886500092</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1.933333333333336</v>
+        <v>3.266374999999992</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>4500</v>
+        <v>-7201.285886500092</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1.966666666666669</v>
+        <v>3.299705357142849</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>3600</v>
+        <v>-20703.69692368776</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2.000000000000003</v>
+        <v>3.333035714285706</v>
       </c>
       <c r="B60" t="n">
-        <v>900</v>
+        <v>1800.321471625023</v>
       </c>
       <c r="C60" t="n">
-        <v>5400</v>
+        <v>3600.642943250046</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2.033333333333336</v>
+        <v>3.366366071428563</v>
       </c>
       <c r="B61" t="n">
-        <v>-900</v>
+        <v>-1800.321471625023</v>
       </c>
       <c r="C61" t="n">
-        <v>3600</v>
+        <v>6301.12515068758</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2.066666666666669</v>
+        <v>3.39969642857142</v>
       </c>
       <c r="B62" t="n">
-        <v>0</v>
+        <v>900.1607358125112</v>
       </c>
       <c r="C62" t="n">
-        <v>4500</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2.100000000000002</v>
+        <v>3.433026785714277</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>3600</v>
+        <v>8101.446622312601</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2.133333333333336</v>
+        <v>3.466357142857134</v>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>-900.1607358125112</v>
       </c>
       <c r="C64" t="n">
-        <v>-13500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2.166666666666669</v>
+        <v>3.499687499999991</v>
       </c>
       <c r="B65" t="n">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>-24300</v>
+        <v>-15302.73250881269</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2.200000000000002</v>
+        <v>3.533017857142847</v>
       </c>
       <c r="B66" t="n">
-        <v>-900</v>
+        <v>900.1607358125112</v>
       </c>
       <c r="C66" t="n">
-        <v>3600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2.233333333333335</v>
+        <v>3.566348214285704</v>
       </c>
       <c r="B67" t="n">
-        <v>900</v>
+        <v>-1800.321471625022</v>
       </c>
       <c r="C67" t="n">
-        <v>6300</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2.266666666666668</v>
+        <v>3.599678571428561</v>
       </c>
       <c r="B68" t="n">
-        <v>-900</v>
+        <v>900.1607358125113</v>
       </c>
       <c r="C68" t="n">
-        <v>2700</v>
+        <v>4500.803679062557</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2.300000000000002</v>
+        <v>3.633008928571418</v>
       </c>
       <c r="B69" t="n">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>4500</v>
+        <v>900.1607358125111</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2.333333333333335</v>
+        <v>3.666339285714275</v>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>-1800.321471625023</v>
       </c>
       <c r="C70" t="n">
-        <v>4500</v>
+        <v>-5400.964414875069</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2.366666666666668</v>
+        <v>3.699669642857132</v>
       </c>
       <c r="B71" t="n">
-        <v>-900</v>
+        <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>2.400000000000001</v>
-      </c>
-      <c r="B72" t="n">
-        <v>0</v>
-      </c>
-      <c r="C72" t="n">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>2.433333333333334</v>
-      </c>
-      <c r="B73" t="n">
-        <v>0</v>
-      </c>
-      <c r="C73" t="n">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>2.466666666666668</v>
-      </c>
-      <c r="B74" t="n">
-        <v>900</v>
-      </c>
-      <c r="C74" t="n">
-        <v>-30600</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>2.500000000000001</v>
-      </c>
-      <c r="B75" t="n">
-        <v>0</v>
-      </c>
-      <c r="C75" t="n">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>2.533333333333334</v>
-      </c>
-      <c r="B76" t="n">
-        <v>-900</v>
-      </c>
-      <c r="C76" t="n">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>2.566666666666667</v>
-      </c>
-      <c r="B77" t="n">
-        <v>-1800</v>
-      </c>
-      <c r="C77" t="n">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>2.600000000000001</v>
-      </c>
-      <c r="B78" t="n">
-        <v>-900</v>
-      </c>
-      <c r="C78" t="n">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>2.633333333333334</v>
-      </c>
-      <c r="B79" t="n">
-        <v>-900</v>
-      </c>
-      <c r="C79" t="n">
-        <v>6300</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>2.666666666666667</v>
-      </c>
-      <c r="B80" t="n">
-        <v>900</v>
-      </c>
-      <c r="C80" t="n">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="B81" t="n">
-        <v>-900</v>
-      </c>
-      <c r="C81" t="n">
-        <v>-13500</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Restaurar funciones de análisis teórico y corregir dependencias
-  Restaurar funciones faltantes en utils.py:
  - ajustar_modelo_parabolico()
  - calcular_trayectoria_teorica()
  - calcular_velocidad_teorica()
  - graficar_comparacion_teorica()
  - calcular_metricas_error()

-  Agregar import numpy as np faltante
-  Corregir ruta de video en main.py (PV_5.mp4  PV_1.mp4)
-  Implementar comparación experimental vs teórica completa
-  Agregar métricas de ajuste (R, RMSE, MAE)
-  Resolver problema de segunda gráfica que no aparecía

Ahora el análisis teórico funciona correctamente mostrando:
- Comparación posición X vs tiempo
- Comparación posición Y vs tiempo
- Trayectoria X vs Y
- Velocidades experimentales vs teóricas
- Parámetros del modelo parabólico
- Estadísticas de bondad de ajuste
</commit_message>
<xml_diff>
--- a/resultados/resultados.xlsx
+++ b/resultados/resultados.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,274 +454,274 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.632854545454542</v>
+        <v>1.483499999999998</v>
       </c>
       <c r="B2" t="n">
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>84</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.666181818181815</v>
+        <v>1.515749999999998</v>
       </c>
       <c r="B3" t="n">
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>84</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.699509090909087</v>
+        <v>1.547999999999998</v>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2.73283636363636</v>
+        <v>1.580249999999998</v>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2.766163636363633</v>
+        <v>1.612499999999998</v>
       </c>
       <c r="B6" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="n">
-        <v>61</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.799490909090905</v>
+        <v>1.644749999999998</v>
       </c>
       <c r="B7" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" t="n">
-        <v>61</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.832818181818178</v>
+        <v>1.676999999999998</v>
       </c>
       <c r="B8" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" t="n">
-        <v>58</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.866145454545451</v>
+        <v>1.709249999999998</v>
       </c>
       <c r="B9" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" t="n">
-        <v>58</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.899472727272723</v>
+        <v>1.741499999999998</v>
       </c>
       <c r="B10" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" t="n">
-        <v>61</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2.932799999999996</v>
+        <v>1.773749999999997</v>
       </c>
       <c r="B11" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" t="n">
-        <v>61</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2.966127272727269</v>
+        <v>1.805999999999997</v>
       </c>
       <c r="B12" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C12" t="n">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2.999454545454541</v>
+        <v>1.838249999999997</v>
       </c>
       <c r="B13" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" t="n">
-        <v>70</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3.032781818181814</v>
+        <v>1.870499999999997</v>
       </c>
       <c r="B14" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C14" t="n">
-        <v>86</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3.066109090909086</v>
+        <v>1.902749999999997</v>
       </c>
       <c r="B15" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C15" t="n">
-        <v>86</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.099436363636359</v>
+        <v>1.934999999999997</v>
       </c>
       <c r="B16" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C16" t="n">
-        <v>107</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3.132763636363632</v>
+        <v>1.967249999999997</v>
       </c>
       <c r="B17" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17" t="n">
-        <v>107</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3.166090909090904</v>
+        <v>1.999499999999997</v>
       </c>
       <c r="B18" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C18" t="n">
-        <v>133</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3.199418181818177</v>
+        <v>2.031749999999997</v>
       </c>
       <c r="B19" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C19" t="n">
-        <v>133</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3.23274545454545</v>
+        <v>2.063999999999997</v>
       </c>
       <c r="B20" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C20" t="n">
-        <v>165</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3.266072727272722</v>
+        <v>2.096249999999996</v>
       </c>
       <c r="B21" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C21" t="n">
-        <v>165</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3.299399999999995</v>
+        <v>2.128499999999996</v>
       </c>
       <c r="B22" t="n">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C22" t="n">
-        <v>202</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3.332727272727268</v>
+        <v>2.160749999999996</v>
       </c>
       <c r="B23" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C23" t="n">
-        <v>202</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>3.36605454545454</v>
+        <v>2.192999999999996</v>
       </c>
       <c r="B24" t="n">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="C24" t="n">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3.399381818181813</v>
+        <v>2.225249999999996</v>
       </c>
       <c r="B25" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C25" t="n">
-        <v>244</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3.432709090909086</v>
+        <v>2.257499999999996</v>
       </c>
       <c r="B26" t="n">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C26" t="n">
         <v>290</v>
@@ -729,68 +729,101 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3.466036363636358</v>
+        <v>2.289749999999996</v>
       </c>
       <c r="B27" t="n">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C27" t="n">
-        <v>290</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>3.499363636363631</v>
+        <v>2.321999999999996</v>
       </c>
       <c r="B28" t="n">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C28" t="n">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3.532690909090904</v>
+        <v>2.354249999999996</v>
       </c>
       <c r="B29" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C29" t="n">
-        <v>343</v>
+        <v>389</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3.566018181818176</v>
+        <v>2.386499999999995</v>
       </c>
       <c r="B30" t="n">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C30" t="n">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>3.599345454545449</v>
+        <v>2.418749999999995</v>
       </c>
       <c r="B31" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C31" t="n">
-        <v>391</v>
+        <v>437</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>3.632672727272722</v>
+        <v>2.450999999999995</v>
       </c>
       <c r="B32" t="n">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C32" t="n">
-        <v>356</v>
+        <v>437</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2.483249999999995</v>
+      </c>
+      <c r="B33" t="n">
+        <v>183</v>
+      </c>
+      <c r="C33" t="n">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2.515499999999995</v>
+      </c>
+      <c r="B34" t="n">
+        <v>183</v>
+      </c>
+      <c r="C34" t="n">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2.547749999999995</v>
+      </c>
+      <c r="B35" t="n">
+        <v>183</v>
+      </c>
+      <c r="C35" t="n">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -804,7 +837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -831,7 +864,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.666181818181815</v>
+        <v>1.515749999999998</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -842,18 +875,18 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.699509090909087</v>
+        <v>1.547999999999998</v>
       </c>
       <c r="B3" t="n">
-        <v>180.0327332242226</v>
+        <v>217.0542635658915</v>
       </c>
       <c r="C3" t="n">
-        <v>-420.0763775231861</v>
+        <v>-434.1085271317829</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.73283636363636</v>
+        <v>1.580249999999998</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -864,18 +897,18 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2.766163636363633</v>
+        <v>1.612499999999998</v>
       </c>
       <c r="B5" t="n">
-        <v>240.0436442989634</v>
+        <v>248.062015503876</v>
       </c>
       <c r="C5" t="n">
-        <v>-270.0490998363339</v>
+        <v>-279.0697674418604</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2.799490909090905</v>
+        <v>1.644749999999998</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -886,18 +919,18 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.832818181818178</v>
+        <v>1.676999999999998</v>
       </c>
       <c r="B7" t="n">
-        <v>360.0654664484452</v>
+        <v>403.1007751937984</v>
       </c>
       <c r="C7" t="n">
-        <v>-90.0163666121113</v>
+        <v>-93.02325581395348</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.866145454545451</v>
+        <v>1.709249999999998</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -908,18 +941,18 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.899472727272723</v>
+        <v>1.741499999999998</v>
       </c>
       <c r="B9" t="n">
-        <v>420.0763775231861</v>
+        <v>434.1085271317829</v>
       </c>
       <c r="C9" t="n">
-        <v>90.0163666121113</v>
+        <v>93.02325581395348</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.932799999999996</v>
+        <v>1.773749999999997</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -930,18 +963,18 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2.966127272727269</v>
+        <v>1.805999999999997</v>
       </c>
       <c r="B11" t="n">
-        <v>450.0818330605565</v>
+        <v>465.1162790697674</v>
       </c>
       <c r="C11" t="n">
-        <v>270.0490998363339</v>
+        <v>279.0697674418604</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2.999454545454541</v>
+        <v>1.838249999999997</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -952,18 +985,18 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3.032781818181814</v>
+        <v>1.870499999999997</v>
       </c>
       <c r="B13" t="n">
-        <v>450.0818330605565</v>
+        <v>434.1085271317829</v>
       </c>
       <c r="C13" t="n">
-        <v>480.0872885979269</v>
+        <v>496.1240310077519</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3.066109090909086</v>
+        <v>1.902749999999997</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -974,18 +1007,18 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3.099436363636359</v>
+        <v>1.934999999999997</v>
       </c>
       <c r="B15" t="n">
-        <v>420.0763775231861</v>
+        <v>434.1085271317829</v>
       </c>
       <c r="C15" t="n">
-        <v>630.114566284779</v>
+        <v>651.1627906976744</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.132763636363632</v>
+        <v>1.967249999999997</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -996,18 +1029,18 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3.166090909090904</v>
+        <v>1.999499999999997</v>
       </c>
       <c r="B17" t="n">
-        <v>420.0763775231861</v>
+        <v>465.1162790697674</v>
       </c>
       <c r="C17" t="n">
-        <v>780.1418439716313</v>
+        <v>806.2015503875969</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3.199418181818177</v>
+        <v>2.031749999999997</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -1018,18 +1051,18 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3.23274545454545</v>
+        <v>2.063999999999997</v>
       </c>
       <c r="B19" t="n">
-        <v>390.0709219858156</v>
+        <v>403.1007751937984</v>
       </c>
       <c r="C19" t="n">
-        <v>960.1745771958538</v>
+        <v>992.2480620155038</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3.266072727272722</v>
+        <v>2.096249999999996</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -1040,123 +1073,156 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3.299399999999995</v>
+        <v>2.128499999999996</v>
       </c>
       <c r="B21" t="n">
-        <v>420.0763775231861</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>1110.201854882706</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3.332727272727268</v>
+        <v>2.160749999999996</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>403.1007751937984</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>1147.286821705426</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3.36605454545454</v>
+        <v>2.192999999999996</v>
       </c>
       <c r="B23" t="n">
-        <v>360.0654664484452</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>1260.229132569558</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>3.399381818181813</v>
+        <v>2.225249999999996</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>372.0930232558139</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1302.325581395349</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3.432709090909086</v>
+        <v>2.257499999999996</v>
       </c>
       <c r="B25" t="n">
-        <v>330.0600109110748</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>1380.25095471904</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3.466036363636358</v>
+        <v>2.289749999999996</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>372.0930232558139</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>1457.364341085271</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3.499363636363631</v>
+        <v>2.321999999999996</v>
       </c>
       <c r="B27" t="n">
-        <v>360.0654664484452</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>1590.289143480633</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>3.532690909090904</v>
+        <v>2.354249999999996</v>
       </c>
       <c r="B28" t="n">
-        <v>0</v>
+        <v>341.0852713178294</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>1612.403100775194</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3.566018181818176</v>
+        <v>2.386499999999995</v>
       </c>
       <c r="B29" t="n">
-        <v>330.0600109110748</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>1440.261865793781</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3.599345454545449</v>
+        <v>2.418749999999995</v>
       </c>
       <c r="B30" t="n">
-        <v>0</v>
+        <v>341.0852713178294</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1488.372093023256</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>3.632672727272722</v>
+        <v>2.450999999999995</v>
       </c>
       <c r="B31" t="n">
-        <v>180.0327332242226</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>-1050.190943807965</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2.483249999999995</v>
+      </c>
+      <c r="B32" t="n">
+        <v>217.0542635658915</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-1085.271317829457</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2.515499999999995</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2.547749999999995</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1170,7 +1236,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1197,321 +1263,354 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.699509090909087</v>
+        <v>1.547999999999998</v>
       </c>
       <c r="B2" t="n">
-        <v>5401.964172030684</v>
+        <v>6730.364761733068</v>
       </c>
       <c r="C2" t="n">
-        <v>-12604.5830680716</v>
+        <v>-13460.72952346614</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.73283636363636</v>
+        <v>1.580249999999998</v>
       </c>
       <c r="B3" t="n">
-        <v>-5401.964172030684</v>
+        <v>-6730.364761733068</v>
       </c>
       <c r="C3" t="n">
-        <v>12604.5830680716</v>
+        <v>13460.72952346614</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.766163636363633</v>
+        <v>1.612499999999998</v>
       </c>
       <c r="B4" t="n">
-        <v>7202.618896040911</v>
+        <v>7691.845441980649</v>
       </c>
       <c r="C4" t="n">
-        <v>-8102.946258046025</v>
+        <v>-8653.326122228231</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2.799490909090905</v>
+        <v>1.644749999999998</v>
       </c>
       <c r="B5" t="n">
-        <v>-7202.618896040911</v>
+        <v>-7691.845441980649</v>
       </c>
       <c r="C5" t="n">
-        <v>8102.946258046025</v>
+        <v>8653.326122228231</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2.832818181818178</v>
+        <v>1.676999999999998</v>
       </c>
       <c r="B6" t="n">
-        <v>10803.92834406137</v>
+        <v>12499.24884321856</v>
       </c>
       <c r="C6" t="n">
-        <v>-2700.982086015342</v>
+        <v>-2884.442040742744</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.866145454545451</v>
+        <v>1.709249999999998</v>
       </c>
       <c r="B7" t="n">
-        <v>-10803.92834406137</v>
+        <v>-12499.24884321856</v>
       </c>
       <c r="C7" t="n">
-        <v>2700.982086015342</v>
+        <v>2884.442040742744</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.899472727272723</v>
+        <v>1.741499999999998</v>
       </c>
       <c r="B8" t="n">
-        <v>12604.5830680716</v>
+        <v>13460.72952346614</v>
       </c>
       <c r="C8" t="n">
-        <v>2700.982086015342</v>
+        <v>2884.442040742744</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.932799999999996</v>
+        <v>1.773749999999997</v>
       </c>
       <c r="B9" t="n">
-        <v>-12604.5830680716</v>
+        <v>-13460.72952346614</v>
       </c>
       <c r="C9" t="n">
-        <v>-2700.982086015342</v>
+        <v>-2884.442040742744</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.966127272727269</v>
+        <v>1.805999999999997</v>
       </c>
       <c r="B10" t="n">
-        <v>13504.91043007671</v>
+        <v>14422.21020371372</v>
       </c>
       <c r="C10" t="n">
-        <v>8102.946258046025</v>
+        <v>8653.326122228231</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2.999454545454541</v>
+        <v>1.838249999999997</v>
       </c>
       <c r="B11" t="n">
-        <v>-13504.91043007671</v>
+        <v>-14422.21020371372</v>
       </c>
       <c r="C11" t="n">
-        <v>-8102.946258046025</v>
+        <v>-8653.326122228231</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3.032781818181814</v>
+        <v>1.870499999999997</v>
       </c>
       <c r="B12" t="n">
-        <v>13504.91043007671</v>
+        <v>13460.72952346614</v>
       </c>
       <c r="C12" t="n">
-        <v>14405.23779208182</v>
+        <v>15383.6908839613</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3.066109090909086</v>
+        <v>1.902749999999997</v>
       </c>
       <c r="B13" t="n">
-        <v>-13504.91043007671</v>
+        <v>-13460.72952346614</v>
       </c>
       <c r="C13" t="n">
-        <v>-14405.23779208182</v>
+        <v>-15383.6908839613</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3.099436363636359</v>
+        <v>1.934999999999997</v>
       </c>
       <c r="B14" t="n">
-        <v>12604.5830680716</v>
+        <v>13460.72952346614</v>
       </c>
       <c r="C14" t="n">
-        <v>18906.87460210739</v>
+        <v>20191.0942851992</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3.132763636363632</v>
+        <v>1.967249999999997</v>
       </c>
       <c r="B15" t="n">
-        <v>-12604.5830680716</v>
+        <v>-13460.72952346614</v>
       </c>
       <c r="C15" t="n">
-        <v>-18906.87460210739</v>
+        <v>-20191.0942851992</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.166090909090904</v>
+        <v>1.999499999999997</v>
       </c>
       <c r="B16" t="n">
-        <v>12604.5830680716</v>
+        <v>14422.21020371372</v>
       </c>
       <c r="C16" t="n">
-        <v>23408.51141213296</v>
+        <v>24998.49768643711</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3.199418181818177</v>
+        <v>2.031749999999997</v>
       </c>
       <c r="B17" t="n">
-        <v>-12604.5830680716</v>
+        <v>-14422.21020371372</v>
       </c>
       <c r="C17" t="n">
-        <v>-23408.51141213296</v>
+        <v>-24998.49768643711</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3.23274545454545</v>
+        <v>2.063999999999997</v>
       </c>
       <c r="B18" t="n">
-        <v>11704.25570606648</v>
+        <v>12499.24884321856</v>
       </c>
       <c r="C18" t="n">
-        <v>28810.47558416364</v>
+        <v>30767.3817679226</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3.266072727272722</v>
+        <v>2.096249999999996</v>
       </c>
       <c r="B19" t="n">
-        <v>-11704.25570606648</v>
+        <v>-12499.24884321856</v>
       </c>
       <c r="C19" t="n">
-        <v>-28810.47558416364</v>
+        <v>-30767.3817679226</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3.299399999999995</v>
+        <v>2.128499999999996</v>
       </c>
       <c r="B20" t="n">
-        <v>12604.5830680716</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>33312.11239418921</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3.332727272727268</v>
+        <v>2.160749999999996</v>
       </c>
       <c r="B21" t="n">
-        <v>-12604.5830680716</v>
+        <v>12499.24884321856</v>
       </c>
       <c r="C21" t="n">
-        <v>-33312.11239418921</v>
+        <v>35574.7851691605</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>3.36605454545454</v>
+        <v>2.192999999999996</v>
       </c>
       <c r="B22" t="n">
-        <v>10803.92834406137</v>
+        <v>-12499.24884321856</v>
       </c>
       <c r="C22" t="n">
-        <v>37813.74920421478</v>
+        <v>-35574.7851691605</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3.399381818181813</v>
+        <v>2.225249999999996</v>
       </c>
       <c r="B23" t="n">
-        <v>-10803.92834406137</v>
+        <v>11537.76816297098</v>
       </c>
       <c r="C23" t="n">
-        <v>-37813.74920421478</v>
+        <v>40382.18857039841</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>3.432709090909086</v>
+        <v>2.257499999999996</v>
       </c>
       <c r="B24" t="n">
-        <v>9903.600982056254</v>
+        <v>-11537.76816297098</v>
       </c>
       <c r="C24" t="n">
-        <v>41415.05865223524</v>
+        <v>-40382.18857039841</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3.466036363636358</v>
+        <v>2.289749999999996</v>
       </c>
       <c r="B25" t="n">
-        <v>-9903.600982056254</v>
+        <v>11537.76816297098</v>
       </c>
       <c r="C25" t="n">
-        <v>-41415.05865223524</v>
+        <v>45189.59197163631</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3.499363636363631</v>
+        <v>2.321999999999996</v>
       </c>
       <c r="B26" t="n">
-        <v>10803.92834406137</v>
+        <v>-11537.76816297098</v>
       </c>
       <c r="C26" t="n">
-        <v>47717.35018627104</v>
+        <v>-45189.59197163631</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3.532690909090904</v>
+        <v>2.354249999999996</v>
       </c>
       <c r="B27" t="n">
-        <v>-10803.92834406137</v>
+        <v>10576.28748272339</v>
       </c>
       <c r="C27" t="n">
-        <v>-47717.35018627104</v>
+        <v>49996.99537287423</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>3.566018181818176</v>
+        <v>2.386499999999995</v>
       </c>
       <c r="B28" t="n">
-        <v>9903.600982056254</v>
+        <v>-10576.28748272339</v>
       </c>
       <c r="C28" t="n">
-        <v>43215.71337624547</v>
+        <v>-49996.99537287423</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3.599345454545449</v>
+        <v>2.418749999999995</v>
       </c>
       <c r="B29" t="n">
-        <v>-9903.600982056254</v>
+        <v>10576.28748272339</v>
       </c>
       <c r="C29" t="n">
-        <v>-43215.71337624547</v>
+        <v>46151.0726518839</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3.632672727272722</v>
+        <v>2.450999999999995</v>
       </c>
       <c r="B30" t="n">
-        <v>5401.964172030684</v>
+        <v>-10576.28748272339</v>
       </c>
       <c r="C30" t="n">
-        <v>-31511.45767017899</v>
+        <v>-46151.0726518839</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2.483249999999995</v>
+      </c>
+      <c r="B31" t="n">
+        <v>6730.364761733068</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-33651.82380866534</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2.515499999999995</v>
+      </c>
+      <c r="B32" t="n">
+        <v>-6730.364761733068</v>
+      </c>
+      <c r="C32" t="n">
+        <v>33651.82380866534</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2.547749999999995</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>